<commit_message>
Keels are not working properly yet. Otherwise, seems to be somewhat OK, and seems to show that the whole net rotation discussion is bullshit (as expected)
</commit_message>
<xml_diff>
--- a/notebooks/settings.xlsx
+++ b/notebooks/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AA9D41-6F1A-AF46-8D40-3CAB62DE0867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2CCB63-E280-DB40-820F-EA2A1501F19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{745898CB-6A96-6A42-A7F0-C6C371FC8CE9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{745898CB-6A96-6A42-A7F0-C6C371FC8CE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Notebook 2 - Optimisation" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -112,13 +112,16 @@
   </si>
   <si>
     <t>Continental keels</t>
+  </si>
+  <si>
+    <t>Minimum plate area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,13 +136,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,17 +166,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFE840A-EBCA-594E-AE7A-240FD341AF2D}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,8 +531,9 @@
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -548,8 +572,8 @@
       <c r="B2" t="b">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1.82E+20</v>
+      <c r="C2" s="4">
+        <v>1.8E+20</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -578,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.74E+20</v>
+        <v>1.76E+20</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -587,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>5.8099999999999999E-2</v>
+        <v>5.9799999999999999E-2</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -607,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1.48E+20</v>
+        <v>1.46E+20</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -629,148 +653,148 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
         <v>1.84E+20</v>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.1968</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.22889999999999999</v>
+      <c r="D5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.1847</v>
+      </c>
+      <c r="G5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.47789999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
         <v>1.38E+20</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>5.0200000000000002E-2</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="D6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
         <v>1.76E+20</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.7099999999999999E-2</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.35339999999999999</v>
+      <c r="D7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="G7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.70279999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1.48E+20</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
-        <v>8.0299999999999996E-2</v>
+      <c r="B8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.46E+20</v>
+      </c>
+      <c r="D8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.16470000000000001</v>
+      </c>
+      <c r="G8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.72689999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
         <v>1.38E+20</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1.7100000000000001E-2</v>
-      </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.58230000000000004</v>
+      <c r="D9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2.7699999999999999E-2</v>
+      </c>
+      <c r="G9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.54220000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -780,8 +804,8 @@
       <c r="B10" t="b">
         <v>0</v>
       </c>
-      <c r="C10">
-        <v>1.82E+20</v>
+      <c r="C10" s="4">
+        <v>1.8E+20</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -810,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>1.74E+20</v>
+        <v>1.76E+20</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -819,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1">
-        <v>5.8099999999999999E-2</v>
+        <v>5.9799999999999999E-2</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -839,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>1.48E+20</v>
+        <v>1.46E+20</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -861,32 +885,32 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
         <v>1.84E+20</v>
       </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0.1968</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0.22889999999999999</v>
+      <c r="D13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.1847</v>
+      </c>
+      <c r="G13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.47789999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -896,113 +920,113 @@
       <c r="B14" t="b">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="9">
         <v>1.38E+20</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>5.0200000000000002E-2</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="D14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
         <v>1.76E+20</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2.7099999999999999E-2</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0.35339999999999999</v>
+      <c r="D15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="G15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0.70279999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>1.48E+20</v>
-      </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1">
-        <v>8.0299999999999996E-2</v>
+      <c r="B16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1.46E+20</v>
+      </c>
+      <c r="D16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.16470000000000001</v>
+      </c>
+      <c r="G16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.72689999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
         <v>1.38E+20</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1.7100000000000001E-2</v>
-      </c>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0.58230000000000004</v>
+      <c r="D17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>2.7699999999999999E-2</v>
+      </c>
+      <c r="G17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0.54220000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1015,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7984F9-5B2E-0F42-9830-D8CBB6318A94}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,9 +1056,10 @@
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1062,15 +1087,18 @@
       <c r="I1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>1.38E+20</v>
       </c>
       <c r="D2" t="b">
@@ -1079,7 +1107,7 @@
       <c r="E2" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="G2" t="b">
@@ -1088,18 +1116,21 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>0.58230000000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="4">
+        <v>5100000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1.38E+20</v>
       </c>
       <c r="D3" s="2" t="b">
@@ -1108,7 +1139,7 @@
       <c r="E3" s="2">
         <v>1000</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="G3" s="2" t="b">
@@ -1117,27 +1148,30 @@
       <c r="H3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>0.58230000000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="4">
+        <v>5100000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1.38E+20</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="E4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="G4" s="2" t="b">
@@ -1146,27 +1180,30 @@
       <c r="H4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>0.58230000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="4">
+        <v>5100000000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1.38E+20</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="G5" s="2" t="b">
@@ -1175,18 +1212,21 @@
       <c r="H5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>0.58230000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="4">
+        <v>5100000000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1.38E+20</v>
       </c>
       <c r="D6" s="2" t="b">
@@ -1195,7 +1235,7 @@
       <c r="E6" s="2">
         <v>1000</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="G6" s="2" t="b">
@@ -1204,18 +1244,21 @@
       <c r="H6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>0.58230000000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="4">
+        <v>5100000000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>1.38E+20</v>
       </c>
       <c r="D7" s="2" t="b">
@@ -1224,7 +1267,7 @@
       <c r="E7" s="2">
         <v>1000</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="G7" s="2" t="b">
@@ -1233,18 +1276,21 @@
       <c r="H7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>0.58230000000000004</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="4">
+        <v>5100000000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>1.38E+20</v>
       </c>
       <c r="D8" s="2" t="b">
@@ -1253,7 +1299,7 @@
       <c r="E8" s="2">
         <v>1000</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="G8" s="2" t="b">
@@ -1262,18 +1308,21 @@
       <c r="H8" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>0.58230000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="4">
+        <v>5100000000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>1.38E+20</v>
       </c>
       <c r="D9" s="2" t="b">
@@ -1282,7 +1331,7 @@
       <c r="E9" s="2">
         <v>1000</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="G9" s="2" t="b">
@@ -1291,8 +1340,11 @@
       <c r="H9" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>0.58230000000000004</v>
+      </c>
+      <c r="J9" s="4">
+        <v>5100000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>